<commit_message>
6390.T more details, £HRN add info
</commit_message>
<xml_diff>
--- a/6390.T - Kato Works Co.xlsx
+++ b/6390.T - Kato Works Co.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E335522F-7D79-4DCF-91F5-CE0D1E63C44C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9A8808-6891-4E56-8D4A-05E6707D6BF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{C91778FA-7584-48E1-8C8D-C8D7867CB047}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>6390.T</t>
   </si>
@@ -34,23 +34,101 @@
     <t>Kato Works Co, Ltd.</t>
   </si>
   <si>
-    <t>Hasbro: Hasbro is a publicly traded company that owns a number of model train brands, including Lionel, which is one of the best-known and most respected brands in the model train industry. Hasbro is listed on the NASDAQ stock exchange.</t>
-  </si>
-  <si>
-    <t>Hornby plc: Hornby plc is a publicly traded company on the London Stock Exchange that owns Hornby, a well-known UK-based model train brand.</t>
-  </si>
-  <si>
-    <t>Tomy Company, Ltd.: Tomy Company, Ltd. is a publicly traded company on the Tokyo Stock Exchange that owns Bachmann, a US-based model train brand.</t>
-  </si>
-  <si>
-    <t>KATO Works Co., Ltd.: KATO Works Co., Ltd. is a publicly traded company on the Tokyo Stock Exchange that produces model trains and other hobby products under the KATO brand.</t>
+    <t>Stock Snapshot</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Debt</t>
+  </si>
+  <si>
+    <t>Net Cash</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>JPYGBP</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>Founded</t>
+  </si>
+  <si>
+    <t>IPO</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Ratios/Metrics</t>
+  </si>
+  <si>
+    <t>P/B</t>
+  </si>
+  <si>
+    <t>P/S</t>
+  </si>
+  <si>
+    <t>EV/S</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>EV/E</t>
+  </si>
+  <si>
+    <t>ROCE</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>Kimiyasu Kato</t>
+  </si>
+  <si>
+    <t>Manufacture and sale of various machines for lifting and construction industries worldwide.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,21 +143,79 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -87,16 +223,231 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -112,6 +463,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>2859</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="File:Kato works-logo.JPG - Wikimedia Commons">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B73FA857-4A03-437C-91C3-1307DAE37968}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2143125" y="85726"/>
+          <a:ext cx="1200150" cy="402908"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF4473D6-7E9C-4722-B96B-EE0E169E5D51}">
-  <dimension ref="B2:H14"/>
+  <dimension ref="B2:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="A11:XFD14"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -422,39 +839,305 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
+      <c r="H2" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H11" s="2" t="s">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H12" s="2" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H13" s="2" t="s">
+      <c r="C6" s="5">
+        <v>699</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="24">
+        <f>C6*$C$13</f>
+        <v>4.4036999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="H14" s="2" t="s">
+      <c r="C7" s="10">
+        <v>11.72</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C8" s="10">
+        <f>C6*C7</f>
+        <v>8192.2800000000007</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="25">
+        <f t="shared" ref="E8:E12" si="0">C8*$C$13</f>
+        <v>51.611364000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10">
+        <f>C9-C10</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10">
+        <f>C8-C11</f>
+        <v>8192.2800000000007</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="25">
+        <f t="shared" si="0"/>
+        <v>51.611364000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11">
+        <v>6.3E-3</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="26"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="19"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="19"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="20"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="14">
+        <v>1895</v>
+      </c>
+      <c r="D25" s="15"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="15"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="13"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="15"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="15"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="15"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="15"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="17"/>
+      <c r="D40" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>